<commit_message>
Changes to Description and Sprint backlog
</commit_message>
<xml_diff>
--- a/Sprint Chart Generator.xlsx
+++ b/Sprint Chart Generator.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayden Moir\Documents\School of Computer Science\Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\computing\Desktop\Software-Engineering-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC5047CF-D1E8-43CE-A00C-CEDD8F13DCA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D9233C2-2400-4E00-8C2C-225D176510FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="Sprint_Points">Sheet1!$B$5</definedName>
     <definedName name="Sprint_Start_Date">Sheet1!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Sprint Start Date</t>
   </si>
@@ -72,11 +71,23 @@
   <si>
     <t>Expected Average Daily Sprint Points</t>
   </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -161,11 +172,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Example</a:t>
+              <a:t>Sprint 3 - Authorize Spotify</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> and Query  Results</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -246,25 +262,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.857142857142858</c:v>
+                  <c:v>17.142857142857142</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.714285714285715</c:v>
+                  <c:v>14.285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>11.428571428571429</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8.5714285714285712</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.4285714285714288</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2857142857142865</c:v>
+                  <c:v>5.7142857142857135</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1428571428571423</c:v>
+                  <c:v>2.8571428571428577</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -324,22 +340,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>13.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>13.33333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>6.6666670000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>6.6666670000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6.6666670000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -582,6 +598,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -613,6 +630,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -620,7 +638,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1199,16 +1216,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1532,11 +1549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5155E8A2-6FD4-455D-A336-6D0F7BDE75E1}">
-  <dimension ref="A2:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>43767</v>
+        <v>43760</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1568,18 +1585,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>43774</v>
+        <v>43767</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
-        <v>15</v>
+        <f t="shared" ref="E3:E10" si="0">Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
+        <v>20</v>
       </c>
       <c r="F3">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points_Completed)</f>
-        <v>15</v>
+        <f t="shared" ref="F3:G10" si="1">Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points_Completed)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,12 +1611,12 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
-        <v>12.857142857142858</v>
+        <f t="shared" si="0"/>
+        <v>17.142857142857142</v>
       </c>
       <c r="F4">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points_Completed)</f>
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>13.333333333333332</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,18 +1624,17 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
-        <v>10.714285714285715</v>
+        <f t="shared" si="0"/>
+        <v>14.285714285714285</v>
       </c>
       <c r="F5">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points_Completed)</f>
-        <v>9</v>
+        <v>13.33333</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,18 +1643,17 @@
       </c>
       <c r="B6">
         <f>Sprint_Points/Sprint_Length__Days</f>
-        <v>2.1428571428571428</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" si="0"/>
+        <v>11.428571428571429</v>
       </c>
       <c r="F6">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points_Completed)</f>
-        <v>6</v>
+        <v>6.6666670000000003</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1646,12 +1661,11 @@
         <v>4</v>
       </c>
       <c r="E7">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
-        <v>6.4285714285714288</v>
+        <f t="shared" si="0"/>
+        <v>8.5714285714285712</v>
       </c>
       <c r="F7">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points_Completed)</f>
-        <v>3</v>
+        <v>6.6666670000000003</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1659,18 +1673,17 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
-        <v>4.2857142857142865</v>
+        <f t="shared" si="0"/>
+        <v>5.7142857142857135</v>
       </c>
       <c r="F8">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points_Completed)</f>
-        <v>0</v>
+        <v>6.6666670000000003</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,14 +1692,14 @@
       </c>
       <c r="B9">
         <f>Sprint_Points/Completion_Time</f>
-        <v>3</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="D9">
         <v>6</v>
       </c>
       <c r="E9">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
-        <v>2.1428571428571423</v>
+        <f t="shared" si="0"/>
+        <v>2.8571428571428577</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1697,11 +1710,28 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <f>Sprint_Points - (Day_of_the_Sprint * Average_Daily_Sprint_Points)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>